<commit_message>
Adding Verification on Scripts
</commit_message>
<xml_diff>
--- a/Data Files/Add Visitor in Security Management.xlsx
+++ b/Data Files/Add Visitor in Security Management.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -38,30 +38,23 @@
     <t>phone</t>
   </si>
   <si>
-    <t>samwesh@gmail.com</t>
-  </si>
-  <si>
-    <t>Sam</t>
-  </si>
-  <si>
-    <t>Wesh</t>
-  </si>
-  <si>
-    <t>0725167892</t>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>Murimi</t>
+  </si>
+  <si>
+    <t>paulmaina@gmail.com</t>
+  </si>
+  <si>
+    <t>0725165221</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,12 +90,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -448,13 +441,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>

</xml_diff>